<commit_message>
Actualizar código: pruebas de simulacion 04/12/23
</commit_message>
<xml_diff>
--- a/pisa_example/Data_Spain_PISA_2018.xlsx
+++ b/pisa_example/Data_Spain_PISA_2018.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\cafee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\cafee\pisa_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954DD7E4-88D7-48EA-A2A2-50176771FA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E542E4A7-8D04-4193-A393-66520CD73DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,10 +478,13 @@
   <dimension ref="A1:J1048"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F1" sqref="F1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="6" width="11.84375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">

</xml_diff>